<commit_message>
Pridanie smerovaca a prepinaca
</commit_message>
<xml_diff>
--- a/sklad/skladove_zasoby.xlsx
+++ b/sklad/skladove_zasoby.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PeterFrantaIIIC\STUDENTSKY_PROJEKT\sklad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3AD102-8DB2-4302-AF89-77A4533CE9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46E8FD2-4BD9-4B74-8362-CB81081A8756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Počet kusov</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Pigtail U.FL - RSMA/F kábel, 0,2 m</t>
+  </si>
+  <si>
+    <t>Smerovac</t>
+  </si>
+  <si>
+    <t>Prepinac</t>
   </si>
 </sst>
 </file>
@@ -388,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,6 +473,22 @@
         <v>3.7</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>